<commit_message>
change print blank to rtf
</commit_message>
<xml_diff>
--- a/control/docs_templates/order.xlsx
+++ b/control/docs_templates/order.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\control\docs_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\control\docs_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A52143-C271-497B-909A-483830B799A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7DFD19-5593-4F1A-B18D-28AB1407448F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,32 +112,19 @@
     <t xml:space="preserve">** В случае доставки груза в обособленное подразделение ООО " ЕВРАЗИЯ ЛОДЖИСТИК" в г. Санкт-Петербург прибытие на выгрузку в строго указанное время. В противном случае применяются штрафные санкции – 2000 рублей/каждый час опоздания.  </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Чистый кузов, возможность пломбировки, БЕЗ догрузов 
+    <t xml:space="preserve">Перевозчик:              </t>
+  </si>
+  <si>
+    <t>1. Чистый кузов, возможность пломбировки, БЕЗ догрузов 
 2. Водитель гражданин РФ, паспорт с собой, без судимости.
-3. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-        <charset val="204"/>
-      </rPr>
-      <t>Подключиться к системе movizor.ru путем установки приложения Movizor GPS или отправки SMS подтверждения после подписания заявки в течение 1-го часа*</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Перевозчик:              </t>
+3. Подключиться к системе movizor.ru путем установки приложения Movizor GPS или отправки SMS подтверждения после подписания заявки в течение 1-го часа*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,33 +203,36 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -350,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -373,6 +363,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -391,21 +390,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -415,40 +438,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,7 +880,7 @@
   <dimension ref="A5:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A27" sqref="A27:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -907,40 +900,40 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
@@ -955,58 +948,58 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="A9" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="8" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="6" t="s">
         <v>5</v>
       </c>
@@ -1017,375 +1010,375 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="24" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="33"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
     </row>
     <row r="20" spans="1:16" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
     </row>
     <row r="24" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="31"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" s="30"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
       <c r="P30" s="5"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="43">
@@ -1416,11 +1409,6 @@
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D14:J14"/>
     <mergeCell ref="D15:J15"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
@@ -1432,6 +1420,11 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:J9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
print xls form, change adress form
</commit_message>
<xml_diff>
--- a/control/docs_templates/order.xlsx
+++ b/control/docs_templates/order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\control\docs_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7DFD19-5593-4F1A-B18D-28AB1407448F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07B6B35-7FB4-4C1C-87A3-EF709D3E2BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,6 +363,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,9 +414,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,45 +443,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A27" sqref="A27:J40"/>
     </sheetView>
   </sheetViews>
@@ -900,40 +900,40 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="1:10" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
@@ -948,58 +948,58 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="11" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="6" t="s">
         <v>5</v>
       </c>
@@ -1010,405 +1010,378 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="20" t="s">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-    </row>
-    <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:16" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" spans="1:16" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32" t="s">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A27" s="33"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A28" s="33"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A29" s="33"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A30" s="33"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
       <c r="P30" s="5"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A32" s="33"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="33"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="33"/>
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="33"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="33"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="33"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A37:E40"/>
-    <mergeCell ref="F37:J40"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A27:E36"/>
-    <mergeCell ref="F27:J36"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:J22"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D15:J15"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
@@ -1425,6 +1398,33 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A37:E40"/>
+    <mergeCell ref="F37:J40"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A27:E36"/>
+    <mergeCell ref="F27:J36"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="F26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>